<commit_message>
First commit by pooja(31-01-2023)
</commit_message>
<xml_diff>
--- a/exceldata/userdata.xlsx
+++ b/exceldata/userdata.xlsx
@@ -40,10 +40,10 @@
     <t xml:space="preserve">status</t>
   </si>
   <si>
-    <t xml:space="preserve">NS Traders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nisha Shah</t>
+    <t xml:space="preserve">Pooja Traders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pooja Shah</t>
   </si>
   <si>
     <t xml:space="preserve">maninagar</t>
@@ -195,10 +195,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -228,7 +228,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>9928787878</v>
+        <v>9928781111</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
First commit by pooja(24-02-2023)
</commit_message>
<xml_diff>
--- a/exceldata/userdata.xlsx
+++ b/exceldata/userdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t xml:space="preserve">firmname</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t xml:space="preserve">Anand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VP Traders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishal patel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV Traders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pooja patel</t>
   </si>
 </sst>
 </file>
@@ -192,13 +204,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -228,7 +240,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>9928781111</v>
+        <v>9928788888</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -248,7 +260,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>4913599252</v>
+        <v>8888599252</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -268,7 +280,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>9925299999</v>
+        <v>6665299999</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -288,7 +300,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1350000000</v>
+        <v>1355555000</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -308,7 +320,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>9921190000</v>
+        <v>9444440000</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -317,6 +329,46 @@
         <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>4878487500</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>4878487501</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>